<commit_message>
Adding 4 to 1 dual mux
</commit_message>
<xml_diff>
--- a/Hardware/Boards/Keenan_Board_2.0/Parts_List.xlsx
+++ b/Hardware/Boards/Keenan_Board_2.0/Parts_List.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Part</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>Dual 4:1 Muxes</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/nxp/74hc4052d-653/ic-analog-mux-dmux-dual-4-x-1/dp/78R7402</t>
+  </si>
+  <si>
+    <t>Cost/Unit</t>
   </si>
 </sst>
 </file>
@@ -417,19 +426,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="103.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="103.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -437,13 +449,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -453,14 +468,18 @@
       <c r="C2" s="3">
         <v>0.49</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3">
+        <f>(C2*B2)</f>
+        <v>0.49</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -470,34 +489,60 @@
       <c r="C3" s="3">
         <v>24.95</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:D5" si="0">(C3*B3)</f>
+        <v>24.95</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>1</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C5" s="3">
         <v>10.99</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>10.99</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
+    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2"/>
-    <hyperlink ref="D3" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E5" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
Added switch to parts list
</commit_message>
<xml_diff>
--- a/Hardware/Boards/Keenan_Board_2.0/Parts_List.xlsx
+++ b/Hardware/Boards/Keenan_Board_2.0/Parts_List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Part</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Cost/Unit</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9609</t>
+  </si>
+  <si>
+    <t>Power Switch</t>
   </si>
 </sst>
 </file>
@@ -426,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,7 +496,7 @@
         <v>24.95</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D5" si="0">(C3*B3)</f>
+        <f t="shared" ref="D3:D6" si="0">(C3*B3)</f>
         <v>24.95</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -517,36 +523,59 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" s="3">
-        <v>10.99</v>
+        <v>0.75</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
         <v>10.99</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>10.99</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
+    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
         <v>11</v>
+      </c>
+      <c r="C7" s="3">
+        <f>SUM(C2:C6)</f>
+        <v>37.75</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E5" r:id="rId2"/>
+    <hyperlink ref="E6" r:id="rId2"/>
     <hyperlink ref="E3" r:id="rId3"/>
     <hyperlink ref="E4" r:id="rId4"/>
+    <hyperlink ref="E5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added Bluetooth to schematic
</commit_message>
<xml_diff>
--- a/Hardware/Boards/Keenan_Board_2.0/Parts_List.xlsx
+++ b/Hardware/Boards/Keenan_Board_2.0/Parts_List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Part</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>http://www.adafruit.com/products/746</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/11295</t>
+  </si>
+  <si>
+    <t>Digital Temp</t>
   </si>
 </sst>
 </file>
@@ -450,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +524,7 @@
         <v>24.95</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:E7" si="0">(D3*C3)</f>
+        <f t="shared" ref="E3:E8" si="0">(D3*C3)</f>
         <v>24.95</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -558,46 +564,56 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>1</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D7" s="3">
         <v>0.75</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E7" s="3">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>1</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D8" s="3">
         <v>10.99</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E8" s="3">
         <f t="shared" si="0"/>
         <v>10.99</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C8" s="4" t="s">
+    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="3">
-        <f>SUM(D2:D7)</f>
+      <c r="D9" s="3">
+        <f>SUM(D2:D8)</f>
         <v>37.75</v>
       </c>
     </row>
@@ -606,8 +622,8 @@
     <hyperlink ref="F2" r:id="rId1"/>
     <hyperlink ref="F3" r:id="rId2"/>
     <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F6" r:id="rId4"/>
-    <hyperlink ref="F7" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId4"/>
+    <hyperlink ref="F8" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>

<commit_message>
Added some things to BOM
</commit_message>
<xml_diff>
--- a/Hardware/Boards/Keenan_Board_2.0/Parts_List.xlsx
+++ b/Hardware/Boards/Keenan_Board_2.0/Parts_List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Part</t>
   </si>
@@ -48,9 +48,6 @@
     <t>TI Stellaris EK-LM4F120XL</t>
   </si>
   <si>
-    <t>Total:</t>
-  </si>
-  <si>
     <t>Dual 4:1 Muxes</t>
   </si>
   <si>
@@ -66,12 +63,6 @@
     <t>Power Switch</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Have</t>
-  </si>
-  <si>
     <t>GPS</t>
   </si>
   <si>
@@ -82,6 +73,18 @@
   </si>
   <si>
     <t>Digital Temp</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Maxim-Integrated/MAX3077EESA+/?qs=sGAEpiMZZMuobhpKLk3hh6ov3TfCBqZhbNybjDy0atQ%3d</t>
+  </si>
+  <si>
+    <t>Parts We Have</t>
+  </si>
+  <si>
+    <t>RS-485 Transceivers</t>
+  </si>
+  <si>
+    <t>Parts We Don't Have</t>
   </si>
 </sst>
 </file>
@@ -91,7 +94,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,19 +118,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -145,15 +151,13 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -456,177 +460,209 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="103.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="103.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2">
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="D2" s="3">
+      <c r="C3" s="2">
         <v>0.49</v>
       </c>
-      <c r="E2" s="3">
-        <f>(D2*C2)</f>
+      <c r="D3" s="2">
+        <f>(C3*B3)</f>
         <v>0.49</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
+      <c r="B4">
         <v>1</v>
       </c>
-      <c r="D3" s="3">
+      <c r="C4" s="2">
         <v>24.95</v>
       </c>
-      <c r="E3" s="3">
-        <f t="shared" ref="E3:E8" si="0">(D3*C3)</f>
+      <c r="D4" s="2">
+        <f t="shared" ref="D4:D9" si="0">(C4*B4)</f>
         <v>24.95</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="D4" s="3">
+      <c r="C5" s="2">
         <v>0.56999999999999995</v>
       </c>
-      <c r="E4" s="3">
+      <c r="D5" s="2">
         <f t="shared" si="0"/>
         <v>2.2799999999999998</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="C5">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
         <v>1</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="C8" s="2">
         <v>0.75</v>
       </c>
-      <c r="E7" s="3">
+      <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="C8">
+      <c r="B9">
         <v>1</v>
       </c>
-      <c r="D8" s="3">
+      <c r="C9" s="2">
         <v>10.99</v>
       </c>
-      <c r="E8" s="3">
+      <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>10.99</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="3">
-        <f>SUM(D2:D8)</f>
-        <v>37.75</v>
-      </c>
+    <row r="10" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>18</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F7" r:id="rId4"/>
-    <hyperlink ref="F8" r:id="rId5"/>
+    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E4" r:id="rId2"/>
+    <hyperlink ref="E5" r:id="rId3"/>
+    <hyperlink ref="E8" r:id="rId4"/>
+    <hyperlink ref="E9" r:id="rId5"/>
+    <hyperlink ref="E11" r:id="rId6"/>
+    <hyperlink ref="E15" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added a few things to BOM
</commit_message>
<xml_diff>
--- a/Hardware/Boards/Keenan_Board_2.0/Parts_List.xlsx
+++ b/Hardware/Boards/Keenan_Board_2.0/Parts_List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Part</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Parts We Don't Have</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -460,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,75 +501,78 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>5</v>
+      <c r="A3" t="s">
+        <v>7</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" s="2">
-        <v>0.49</v>
+        <v>24.95</v>
       </c>
       <c r="D3" s="2">
-        <f>(C3*B3)</f>
-        <v>0.49</v>
+        <f t="shared" ref="D3:D6" si="0">(C3*B3)</f>
+        <v>24.95</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2">
-        <v>24.95</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" ref="D4:D9" si="0">(C4*B4)</f>
-        <v>24.95</v>
+        <f t="shared" si="0"/>
+        <v>3.42</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="D5" s="2">
-        <f t="shared" si="0"/>
-        <v>2.2799999999999998</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="C6" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
       <c r="E6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -575,91 +581,95 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8">
+      <c r="E8" s="1"/>
+    </row>
+    <row r="10" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="D8" s="2">
-        <f t="shared" si="0"/>
-        <v>0.75</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
         <v>1</v>
       </c>
-      <c r="C9" s="2">
-        <v>10.99</v>
-      </c>
-      <c r="D9" s="2">
-        <f t="shared" si="0"/>
-        <v>10.99</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B10" s="3"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E11" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
-        <v>3</v>
+      <c r="C14" s="2">
+        <v>0.49</v>
+      </c>
+      <c r="D14" s="2">
+        <f>(C14*B14)</f>
+        <v>0.49</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B15">
-        <v>18</v>
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>10.99</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" ref="D15" si="1">(C15*B15)</f>
+        <v>10.99</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="E4" r:id="rId2"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="E8" r:id="rId4"/>
-    <hyperlink ref="E9" r:id="rId5"/>
-    <hyperlink ref="E11" r:id="rId6"/>
-    <hyperlink ref="E15" r:id="rId7"/>
+    <hyperlink ref="E14" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E6" r:id="rId4"/>
+    <hyperlink ref="E12" r:id="rId5"/>
+    <hyperlink ref="E15" r:id="rId6"/>
+    <hyperlink ref="E7" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>

</xml_diff>